<commit_message>
fix: filter invalid items in eu funds basic packet
</commit_message>
<xml_diff>
--- a/reports/european_funds_requests/templates/xlsx/template.xlsx
+++ b/reports/european_funds_requests/templates/xlsx/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgelg/git/yssb-devi-reports/reports/european_funds_requests/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D81705-D83D-5D41-A867-E10854000C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D533585D-44CB-3B45-8D70-A13E53939130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30760" yWindow="5180" windowWidth="32080" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -408,16 +408,16 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1" outlineLevel="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="6" width="17.5" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="6" width="17.5" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="18.5" bestFit="1" customWidth="1"/>
@@ -430,34 +430,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
fix: add domain field in EU funds report
</commit_message>
<xml_diff>
--- a/reports/european_funds_requests/templates/xlsx/template.xlsx
+++ b/reports/european_funds_requests/templates/xlsx/template.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgelg/git/yssb-devi-reports/reports/european_funds_requests/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D533585D-44CB-3B45-8D70-A13E53939130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCADA8F-E8A3-3840-BAA1-41FA287669E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$M$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Request ID</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Technical Email</t>
+  </si>
+  <si>
+    <t>Domain</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -421,11 +424,11 @@
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5" customWidth="1"/>
-    <col min="12" max="12" width="22.5" customWidth="1"/>
+    <col min="11" max="12" width="18.5" customWidth="1"/>
+    <col min="13" max="13" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,9 +465,12 @@
       <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
+  <autoFilter ref="A1:M1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: add domain field in EU funds report (#13)
</commit_message>
<xml_diff>
--- a/reports/european_funds_requests/templates/xlsx/template.xlsx
+++ b/reports/european_funds_requests/templates/xlsx/template.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgelg/git/yssb-devi-reports/reports/european_funds_requests/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D533585D-44CB-3B45-8D70-A13E53939130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCADA8F-E8A3-3840-BAA1-41FA287669E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$M$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Request ID</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Technical Email</t>
+  </si>
+  <si>
+    <t>Domain</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -421,11 +424,11 @@
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5" customWidth="1"/>
-    <col min="12" max="12" width="22.5" customWidth="1"/>
+    <col min="11" max="12" width="18.5" customWidth="1"/>
+    <col min="13" max="13" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,9 +465,12 @@
       <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
+  <autoFilter ref="A1:M1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(PYME-4265): Add subscription id in excel
</commit_message>
<xml_diff>
--- a/reports/european_funds_requests/templates/xlsx/template.xlsx
+++ b/reports/european_funds_requests/templates/xlsx/template.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgelg/git/yssb-devi-reports/reports/european_funds_requests/templates/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cx02538/Telefonica/yssb-devi-reports/reports/european_funds_requests/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCADA8F-E8A3-3840-BAA1-41FA287669E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5B6E1E-B3A8-3247-B7E2-77FC376BDB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Request ID</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Domain</t>
+  </si>
+  <si>
+    <t>Subscription ID</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -423,12 +426,13 @@
     <col min="5" max="6" width="17.5" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.5" customWidth="1"/>
-    <col min="13" max="13" width="22.5" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="11" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="18.5" customWidth="1"/>
+    <col min="14" max="14" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,23 +458,26 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
+  <autoFilter ref="A1:N1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(PYME-4265): Add subscription id in excel (#22)
</commit_message>
<xml_diff>
--- a/reports/european_funds_requests/templates/xlsx/template.xlsx
+++ b/reports/european_funds_requests/templates/xlsx/template.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgelg/git/yssb-devi-reports/reports/european_funds_requests/templates/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cx02538/Telefonica/yssb-devi-reports/reports/european_funds_requests/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCADA8F-E8A3-3840-BAA1-41FA287669E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5B6E1E-B3A8-3247-B7E2-77FC376BDB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Request ID</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Domain</t>
+  </si>
+  <si>
+    <t>Subscription ID</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -423,12 +426,13 @@
     <col min="5" max="6" width="17.5" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.5" customWidth="1"/>
-    <col min="13" max="13" width="22.5" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="11" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="18.5" customWidth="1"/>
+    <col min="14" max="14" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,23 +458,26 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
+  <autoFilter ref="A1:N1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "feat(PYME-4265): Add subscription id in excel"
This reverts commit d920faaf007ab035dfb3d6a7884faeb4dda07717.
</commit_message>
<xml_diff>
--- a/reports/european_funds_requests/templates/xlsx/template.xlsx
+++ b/reports/european_funds_requests/templates/xlsx/template.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cx02538/Telefonica/yssb-devi-reports/reports/european_funds_requests/templates/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgelg/git/yssb-devi-reports/reports/european_funds_requests/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5B6E1E-B3A8-3247-B7E2-77FC376BDB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCADA8F-E8A3-3840-BAA1-41FA287669E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$M$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Request ID</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>Domain</t>
-  </si>
-  <si>
-    <t>Subscription ID</t>
   </si>
 </sst>
 </file>
@@ -411,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -426,13 +423,12 @@
     <col min="5" max="6" width="17.5" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="11" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="18.5" customWidth="1"/>
-    <col min="14" max="14" width="22.5" customWidth="1"/>
+    <col min="9" max="10" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="18.5" customWidth="1"/>
+    <col min="13" max="13" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,26 +454,23 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
+  <autoFilter ref="A1:M1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(PYME-4531): Add approved date in european_funds_request
</commit_message>
<xml_diff>
--- a/reports/european_funds_requests/templates/xlsx/template.xlsx
+++ b/reports/european_funds_requests/templates/xlsx/template.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgelg/git/yssb-devi-reports/reports/european_funds_requests/templates/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cx02538/Telefonica/yssb-devi-reports/reports/european_funds_requests/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCADA8F-E8A3-3840-BAA1-41FA287669E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C747B16D-5FE4-7A45-AD5F-B4E596AA1443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Request ID</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Domain</t>
+  </si>
+  <si>
+    <t>Approved At</t>
   </si>
 </sst>
 </file>
@@ -408,27 +411,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="6" width="17.5" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.5" customWidth="1"/>
-    <col min="13" max="13" width="22.5" customWidth="1"/>
+    <col min="3" max="4" width="19.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="7" width="17.5" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="18.5" customWidth="1"/>
+    <col min="14" max="14" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,38 +442,41 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
+  <autoFilter ref="A1:N1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(PYME-4531): Add approved date in european_funds_request (#26)
* feat(PYME-4531): Add approved date in european_funds_request

* Remove approved date
</commit_message>
<xml_diff>
--- a/reports/european_funds_requests/templates/xlsx/template.xlsx
+++ b/reports/european_funds_requests/templates/xlsx/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgelg/git/yssb-devi-reports/reports/european_funds_requests/templates/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cx02538/Telefonica/yssb-devi-reports/reports/european_funds_requests/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCADA8F-E8A3-3840-BAA1-41FA287669E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD62E42A-76D6-074A-982B-DF69352FF631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -411,7 +411,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>

</xml_diff>